<commit_message>
Updated with plan for Sprint 4
</commit_message>
<xml_diff>
--- a/11. Sprint Planning and Review/Sprint 4 (03 - 10 May 2020)/Sprint 4 Burndown Chart.xlsx
+++ b/11. Sprint Planning and Review/Sprint 4 (03 - 10 May 2020)/Sprint 4 Burndown Chart.xlsx
@@ -5,18 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/804ce03f3a9950f7/Documents/MSSA/01. San Diego (Cloud Application Developer)/03. CAD Project/11. Sprint Planning and Review/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/804ce03f3a9950f7/Documents/MSSA/01. San Diego (Cloud Application Developer)/03. CAD Project/11. Sprint Planning and Review/Sprint 4 (03 - 10 May 2020)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{134F216F-0543-425F-9084-9581F4C35571}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{797B9716-597C-4400-99A8-C31BB735D239}"/>
+  <xr:revisionPtr revIDLastSave="99" documentId="8_{134F216F-0543-425F-9084-9581F4C35571}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FF6D0E77-1E2B-4BCE-888B-D02DD801AB7B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AE03FF15-3D1E-4EC4-9438-EDE4E738FADC}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sprint 3" sheetId="2" r:id="rId1"/>
-    <sheet name="Sprint 2" sheetId="1" r:id="rId2"/>
+    <sheet name="Sprint 4" sheetId="4" r:id="rId1"/>
+    <sheet name="Sprint 3" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint 2" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" calcCompleted="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -61,6 +62,9 @@
   </si>
   <si>
     <t>Sprint 3: 26 April - 03 May 2020</t>
+  </si>
+  <si>
+    <t>Sprint 4: 03 - 10 May 2020</t>
   </si>
 </sst>
 </file>
@@ -131,11 +135,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -172,6 +179,734 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Sprint 4 Burndown Chart </a:t>
+            </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>(as of  04MAY2020)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 4'!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual Tasks Remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 4'!$A$4:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>43954</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43955</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43956</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43957</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43958</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43959</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43960</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43961</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 4'!$D$4:$D$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B14D-462E-85AB-CB83B87F76D9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 4'!$F$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ideal # Remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Sprint 4'!$A$4:$A$11</c:f>
+              <c:numCache>
+                <c:formatCode>d\-mmm\-yy</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>43954</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43955</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43956</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>43957</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>43958</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>43959</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>43960</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43961</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 4'!$F$4:$F$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B14D-462E-85AB-CB83B87F76D9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Sprint 4'!$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tasks Added</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="17"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="dk1">
+                          <a:lumMod val="50000"/>
+                          <a:lumOff val="50000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>'Sprint 4'!$C$4:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B14D-462E-85AB-CB83B87F76D9}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="464920008"/>
+        <c:axId val="464919024"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="464920008"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="d\-mmm\-yy" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="dk1">
+                    <a:lumMod val="75000"/>
+                    <a:lumOff val="25000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="464919024"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="464919024"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:gradFill>
+                <a:gsLst>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="95000"/>
+                      <a:lumOff val="5000"/>
+                      <a:alpha val="42000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="0">
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="75000"/>
+                      <a:alpha val="36000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="464920008"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="39000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="39000">
+          <a:schemeClr val="lt1"/>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="lt1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="25000"/>
+          <a:lumOff val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -914,7 +1649,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1525,13 +2260,10 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="13">
+  <a:schemeClr val="accent6"/>
+  <a:schemeClr val="accent5"/>
   <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
   <cs:variation/>
   <cs:variation>
     <a:lumMod val="60000"/>
@@ -1604,6 +2336,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="228">
   <cs:axisTitle>
@@ -2740,7 +3512,618 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="228">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200" cap="all" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="39000">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+          <a:alpha val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:alpha val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="17"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+                <a:alpha val="42000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="0">
+              <a:schemeClr val="lt1">
+                <a:lumMod val="75000"/>
+                <a:alpha val="36000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="95000"/>
+          <a:alpha val="39000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="31750" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>933449</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>80961</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1057274</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88465B0D-4B01-46A8-85A3-B6210BDFE5CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2783,7 +4166,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3120,10 +4503,232 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44963027-8C8D-493D-B906-11564E8A507A}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="10">
+        <v>8</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>43954</v>
+      </c>
+      <c r="B4" s="7">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7">
+        <f>$D$2+SUM(C4)-SUM(B4)</f>
+        <v>8</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7">
+        <f>D2</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>43955</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7">
+        <f>$D$2+SUM(C4:C5)-SUM(B4:B5)</f>
+        <v>8</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="7">
+        <f>$D$2-SUM(E4:E5)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>43956</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7">
+        <f>$D$2+SUM(C4:C6)-SUM(B4:B6)</f>
+        <v>8</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7">
+        <f>$D$2-SUM(E4:E6)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>43957</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7">
+        <f>$D$2+SUM(C4:C7)-SUM(B4:B7)</f>
+        <v>8</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7">
+        <f>$D$2-SUM(E4:E7)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>43958</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7">
+        <f>$D$2+SUM(C4:C8)-SUM(B4:B8)</f>
+        <v>8</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7">
+        <f>$D$2-SUM(E4:E8)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>43959</v>
+      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7">
+        <f>$D$2+SUM(C4:C9)-SUM(B4:B9)</f>
+        <v>8</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7">
+        <f>$D$2-SUM(E4:E9)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>43960</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7">
+        <f>$D$2+SUM(C4:C10)-SUM(B4:B10)</f>
+        <v>8</v>
+      </c>
+      <c r="E10" s="7">
+        <v>1</v>
+      </c>
+      <c r="F10" s="7">
+        <f>$D$2-SUM(E4:E10)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>43961</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="7">
+        <f>$D$2+SUM(C4:C11)-SUM(B4:B11)</f>
+        <v>8</v>
+      </c>
+      <c r="E11" s="7">
+        <f t="shared" ref="E5:E11" si="0">_xlfn.CEILING.MATH(($D$2/7),1)</f>
+        <v>2</v>
+      </c>
+      <c r="F11" s="7">
+        <f>$D$2-SUM(E4:E11)</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:F2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D9F7AC-EB77-438E-9CB2-3FFA9A4E9929}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
@@ -3139,26 +4744,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="10">
         <v>6</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -3370,7 +4975,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC187263-BB50-456B-8121-FD748AE814DF}">
   <dimension ref="A1:F11"/>
   <sheetViews>
@@ -3390,26 +4995,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="9">
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="10">
         <v>5</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">

</xml_diff>

<commit_message>
Added review products from Sprint 4 and planned Sprint 5
</commit_message>
<xml_diff>
--- a/11. Sprint Planning and Review/Sprint 4 (03 - 10 May 2020)/Sprint 4 Burndown Chart.xlsx
+++ b/11. Sprint Planning and Review/Sprint 4 (03 - 10 May 2020)/Sprint 4 Burndown Chart.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/804ce03f3a9950f7/Documents/MSSA/01. San Diego (Cloud Application Developer)/03. CAD Project/11. Sprint Planning and Review/Sprint 4 (03 - 10 May 2020)/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="99" documentId="8_{134F216F-0543-425F-9084-9581F4C35571}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FF6D0E77-1E2B-4BCE-888B-D02DD801AB7B}"/>
+  <xr:revisionPtr revIDLastSave="115" documentId="8_{134F216F-0543-425F-9084-9581F4C35571}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{2BB1329B-454F-468D-8D57-B2264F7CA655}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AE03FF15-3D1E-4EC4-9438-EDE4E738FADC}"/>
   </bookViews>
@@ -222,7 +222,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>(as of  04MAY2020)</a:t>
+              <a:t>(as of  09MAY2020)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -407,13 +407,13 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -685,6 +685,27 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -4506,8 +4527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44963027-8C8D-493D-B906-11564E8A507A}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4589,8 +4610,12 @@
       <c r="A5" s="3">
         <v>43955</v>
       </c>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
+      <c r="B5" s="7">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0</v>
+      </c>
       <c r="D5" s="7">
         <f>$D$2+SUM(C4:C5)-SUM(B4:B5)</f>
         <v>8</v>
@@ -4607,8 +4632,12 @@
       <c r="A6" s="3">
         <v>43956</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
+      <c r="B6" s="7">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0</v>
+      </c>
       <c r="D6" s="7">
         <f>$D$2+SUM(C4:C6)-SUM(B4:B6)</f>
         <v>8</v>
@@ -4625,8 +4654,12 @@
       <c r="A7" s="3">
         <v>43957</v>
       </c>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
+      <c r="B7" s="7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0</v>
+      </c>
       <c r="D7" s="7">
         <f>$D$2+SUM(C4:C7)-SUM(B4:B7)</f>
         <v>8</v>
@@ -4643,8 +4676,12 @@
       <c r="A8" s="3">
         <v>43958</v>
       </c>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
+      <c r="B8" s="7">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0</v>
+      </c>
       <c r="D8" s="7">
         <f>$D$2+SUM(C4:C8)-SUM(B4:B8)</f>
         <v>8</v>
@@ -4661,11 +4698,15 @@
       <c r="A9" s="3">
         <v>43959</v>
       </c>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
+      <c r="B9" s="7">
+        <v>2</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0</v>
+      </c>
       <c r="D9" s="7">
         <f>$D$2+SUM(C4:C9)-SUM(B4:B9)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E9" s="7">
         <v>1</v>
@@ -4679,11 +4720,15 @@
       <c r="A10" s="3">
         <v>43960</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
+      <c r="B10" s="7">
+        <v>2</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0</v>
+      </c>
       <c r="D10" s="7">
         <f>$D$2+SUM(C4:C10)-SUM(B4:B10)</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E10" s="7">
         <v>1</v>
@@ -4697,14 +4742,18 @@
       <c r="A11" s="3">
         <v>43961</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7"/>
+      <c r="B11" s="7">
+        <v>0</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0</v>
+      </c>
       <c r="D11" s="7">
         <f>$D$2+SUM(C4:C11)-SUM(B4:B11)</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="E11" s="7">
-        <f t="shared" ref="E5:E11" si="0">_xlfn.CEILING.MATH(($D$2/7),1)</f>
+        <f t="shared" ref="E11" si="0">_xlfn.CEILING.MATH(($D$2/7),1)</f>
         <v>2</v>
       </c>
       <c r="F11" s="7">

</xml_diff>